<commit_message>
proofing through ms word
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -146,8 +146,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:alpha val="36000"/>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="75000"/>
+                <a:alpha val="54000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:ln>
@@ -784,16 +785,79 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="262638224"/>
-        <c:axId val="262635424"/>
+        <c:axId val="112158752"/>
+        <c:axId val="112159312"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="262638224"/>
+        <c:axId val="112158752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Day</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.5573733353193433"/>
+              <c:y val="0.78192888385593473"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -830,7 +894,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="262635424"/>
+        <c:crossAx val="112159312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -838,7 +902,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="262635424"/>
+        <c:axId val="112159312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -858,6 +922,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tweet count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -889,7 +1009,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="262638224"/>
+        <c:crossAx val="112158752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -903,7 +1023,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.19555031065200659"/>
+          <c:y val="4.1340982363457408E-2"/>
+          <c:w val="0.75250798758171822"/>
+          <c:h val="8.1728137617258903E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1535,16 +1664,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>100012</xdr:colOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>404812</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>42862</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2152,8 +2281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:AH6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AK5" sqref="AK5"/>
+    <sheetView tabSelected="1" topLeftCell="Y6" workbookViewId="0">
+      <selection activeCell="AN21" sqref="AN21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
presentation final review:eirini: into/relworks
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="statistics" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
     <t>Positive</t>
   </si>
   <si>
-    <t>Nagative</t>
+    <t>Negative</t>
   </si>
 </sst>
 </file>
@@ -791,11 +791,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="199423280"/>
-        <c:axId val="199423840"/>
+        <c:axId val="171576816"/>
+        <c:axId val="171577376"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="199423280"/>
+        <c:axId val="171576816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -900,7 +900,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199423840"/>
+        <c:crossAx val="171577376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -908,7 +908,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="199423840"/>
+        <c:axId val="171577376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -954,7 +954,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1015,7 +1014,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199423280"/>
+        <c:crossAx val="171576816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1260,7 +1259,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Nagative</c:v>
+                  <c:v>Negative</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1385,11 +1384,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="257278304"/>
-        <c:axId val="257279424"/>
+        <c:axId val="171581296"/>
+        <c:axId val="171581856"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="257278304"/>
+        <c:axId val="171581296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1431,7 +1430,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257279424"/>
+        <c:crossAx val="171581856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1439,7 +1438,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="257279424"/>
+        <c:axId val="171581856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1490,7 +1489,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257278304"/>
+        <c:crossAx val="171581296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3344,8 +3343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:AH10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:AH10"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AD20" sqref="AD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>